<commit_message>
Updated USA-ENG match events
</commit_message>
<xml_diff>
--- a/source/excel/shebelieves-cup-2016/shebelieves-cup-2016-usa-eng-030316.xlsx
+++ b/source/excel/shebelieves-cup-2016/shebelieves-cup-2016-usa-eng-030316.xlsx
@@ -2580,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XEQ1458"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1437" workbookViewId="0">
-      <selection activeCell="C1453" sqref="C1453"/>
+    <sheetView tabSelected="1" topLeftCell="A1410" workbookViewId="0">
+      <selection activeCell="I1417" sqref="I1417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -51925,7 +51925,7 @@
         <v>40</v>
       </c>
       <c r="G822" s="4" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="I822" s="40" t="s">
         <v>81</v>
@@ -69265,7 +69265,7 @@
         <v>40</v>
       </c>
       <c r="G1111" s="4" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="I1111" s="40" t="s">
         <v>20</v>

</xml_diff>